<commit_message>
keep unknown in the output files
</commit_message>
<xml_diff>
--- a/Multi-taxa_data/PLITs/2-Relative_cover_category/rel_cov_input.xlsx
+++ b/Multi-taxa_data/PLITs/2-Relative_cover_category/rel_cov_input.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V70"/>
+  <dimension ref="A1:X70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,45 +425,55 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>unknown</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>zoanthids</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>sd_alg</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>sd_boulder</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>sd_hc</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>sd_other</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>sd_rubble</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>sd_sand</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>sd_softc</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>sd_unknown</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>sd_zoanth</t>
         </is>
@@ -501,7 +511,7 @@
         </is>
       </c>
       <c r="G2">
-        <v>0.852</v>
+        <v>0.85</v>
       </c>
       <c r="H2">
         <v>0.018</v>
@@ -513,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.06</v>
+        <v>0.059</v>
       </c>
       <c r="L2">
         <v>0.047</v>
@@ -522,30 +532,36 @@
         <v>0.023</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
         <v>0.05</v>
       </c>
-      <c r="P2">
-        <v>0.01</v>
-      </c>
       <c r="Q2">
         <v>0.01</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>0.03</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>0.02</v>
       </c>
-      <c r="U2">
-        <v>0.01</v>
-      </c>
       <c r="V2">
+        <v>0.01</v>
+      </c>
+      <c r="W2">
+        <v>0.01</v>
+      </c>
+      <c r="X2">
         <v>0</v>
       </c>
     </row>
@@ -581,13 +597,13 @@
         </is>
       </c>
       <c r="G3">
-        <v>0.9330000000000001</v>
+        <v>0.92</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="J3">
         <v>0.001</v>
@@ -596,36 +612,42 @@
         <v>0.004</v>
       </c>
       <c r="L3">
-        <v>0.043</v>
+        <v>0.042</v>
       </c>
       <c r="M3">
         <v>0.001</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>0.014</v>
       </c>
       <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
         <v>0.05</v>
       </c>
-      <c r="P3">
-        <v>0.01</v>
-      </c>
       <c r="Q3">
         <v>0.01</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>0.03</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>0.02</v>
       </c>
-      <c r="U3">
-        <v>0.01</v>
-      </c>
       <c r="V3">
+        <v>0.01</v>
+      </c>
+      <c r="W3">
+        <v>0.01</v>
+      </c>
+      <c r="X3">
         <v>0</v>
       </c>
     </row>
@@ -661,7 +683,7 @@
         </is>
       </c>
       <c r="G4">
-        <v>0.943</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="H4">
         <v>0.01</v>
@@ -673,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="L4">
         <v>0.006</v>
@@ -682,30 +704,36 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
         <v>0.05</v>
       </c>
-      <c r="P4">
-        <v>0.01</v>
-      </c>
       <c r="Q4">
         <v>0.01</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>0.03</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>0.02</v>
       </c>
-      <c r="U4">
-        <v>0.01</v>
-      </c>
       <c r="V4">
+        <v>0.01</v>
+      </c>
+      <c r="W4">
+        <v>0.01</v>
+      </c>
+      <c r="X4">
         <v>0</v>
       </c>
     </row>
@@ -741,7 +769,7 @@
         </is>
       </c>
       <c r="G5">
-        <v>0.954</v>
+        <v>0.953</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -762,30 +790,36 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
         <v>0.04</v>
       </c>
-      <c r="P5">
-        <v>0.01</v>
-      </c>
       <c r="Q5">
+        <v>0.01</v>
+      </c>
+      <c r="R5">
         <v>0.03</v>
       </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
       <c r="S5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>0.01</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>0</v>
       </c>
     </row>
@@ -821,13 +855,13 @@
         </is>
       </c>
       <c r="G6">
-        <v>0.878</v>
+        <v>0.874</v>
       </c>
       <c r="H6">
         <v>0.023</v>
       </c>
       <c r="I6">
-        <v>0.074</v>
+        <v>0.073</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -842,30 +876,36 @@
         <v>0.001</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>0.04</v>
       </c>
-      <c r="P6">
-        <v>0.01</v>
-      </c>
       <c r="Q6">
+        <v>0.01</v>
+      </c>
+      <c r="R6">
         <v>0.03</v>
       </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
       <c r="S6">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>0.01</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>0</v>
       </c>
     </row>
@@ -901,7 +941,7 @@
         </is>
       </c>
       <c r="G7">
-        <v>0.902</v>
+        <v>0.899</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -925,27 +965,33 @@
         <v>0.003</v>
       </c>
       <c r="O7">
+        <v>0.003</v>
+      </c>
+      <c r="P7">
         <v>0.04</v>
       </c>
-      <c r="P7">
-        <v>0.01</v>
-      </c>
       <c r="Q7">
+        <v>0.01</v>
+      </c>
+      <c r="R7">
         <v>0.03</v>
       </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
       <c r="S7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <v>0.01</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
         <v>0</v>
       </c>
     </row>
@@ -981,13 +1027,13 @@
         </is>
       </c>
       <c r="G8">
-        <v>0.508</v>
+        <v>0.497</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0.106</v>
+        <v>0.104</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -996,36 +1042,42 @@
         <v>0.005</v>
       </c>
       <c r="L8">
-        <v>0.098</v>
+        <v>0.096</v>
       </c>
       <c r="M8">
-        <v>0.283</v>
+        <v>0.276</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>0.13</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>0.03</v>
       </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
       <c r="S8">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T8">
+        <v>0.01</v>
+      </c>
+      <c r="U8">
         <v>0.04</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>0.11</v>
       </c>
-      <c r="V8">
+      <c r="W8">
+        <v>0.01</v>
+      </c>
+      <c r="X8">
         <v>0</v>
       </c>
     </row>
@@ -1061,51 +1113,57 @@
         </is>
       </c>
       <c r="G9">
-        <v>0.698</v>
+        <v>0.691</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.144</v>
+        <v>0.143</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="L9">
-        <v>0.037</v>
+        <v>0.036</v>
       </c>
       <c r="M9">
-        <v>0.108</v>
+        <v>0.107</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>0.13</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
       <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
         <v>0.03</v>
       </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
       <c r="S9">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T9">
+        <v>0.01</v>
+      </c>
+      <c r="U9">
         <v>0.04</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>0.11</v>
       </c>
-      <c r="V9">
+      <c r="W9">
+        <v>0.01</v>
+      </c>
+      <c r="X9">
         <v>0</v>
       </c>
     </row>
@@ -1141,13 +1199,13 @@
         </is>
       </c>
       <c r="G10">
-        <v>0.752</v>
+        <v>0.734</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.155</v>
+        <v>0.152</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1156,36 +1214,42 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="M10">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>0.024</v>
       </c>
       <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
         <v>0.13</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
       <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <v>0.03</v>
       </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
       <c r="S10">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T10">
+        <v>0.01</v>
+      </c>
+      <c r="U10">
         <v>0.04</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>0.11</v>
       </c>
-      <c r="V10">
+      <c r="W10">
+        <v>0.01</v>
+      </c>
+      <c r="X10">
         <v>0</v>
       </c>
     </row>
@@ -1221,13 +1285,13 @@
         </is>
       </c>
       <c r="G11">
-        <v>0.827</v>
+        <v>0.8</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.173</v>
+        <v>0.167</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1242,20 +1306,20 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.033</v>
       </c>
       <c r="O11">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
         <v>0.08</v>
       </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
       <c r="S11">
         <v>0</v>
       </c>
@@ -1263,9 +1327,15 @@
         <v>0</v>
       </c>
       <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
         <v>0.03</v>
       </c>
-      <c r="V11">
+      <c r="W11">
+        <v>0.01</v>
+      </c>
+      <c r="X11">
         <v>0.12</v>
       </c>
     </row>
@@ -1301,13 +1371,13 @@
         </is>
       </c>
       <c r="G12">
-        <v>0.6840000000000001</v>
+        <v>0.672</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0.265</v>
+        <v>0.26</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1322,20 +1392,20 @@
         <v>0.013</v>
       </c>
       <c r="N12">
+        <v>0.017</v>
+      </c>
+      <c r="O12">
         <v>0.038</v>
       </c>
-      <c r="O12">
-        <v>0.11</v>
-      </c>
       <c r="P12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
         <v>0.08</v>
       </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
       <c r="S12">
         <v>0</v>
       </c>
@@ -1343,9 +1413,15 @@
         <v>0</v>
       </c>
       <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
         <v>0.03</v>
       </c>
-      <c r="V12">
+      <c r="W12">
+        <v>0.01</v>
+      </c>
+      <c r="X12">
         <v>0.12</v>
       </c>
     </row>
@@ -1381,7 +1457,7 @@
         </is>
       </c>
       <c r="G13">
-        <v>0.613</v>
+        <v>0.61</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1402,20 +1478,20 @@
         <v>0.052</v>
       </c>
       <c r="N13">
-        <v>0.227</v>
+        <v>0.006</v>
       </c>
       <c r="O13">
-        <v>0.11</v>
+        <v>0.226</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>0.08</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
       <c r="S13">
         <v>0</v>
       </c>
@@ -1423,9 +1499,15 @@
         <v>0</v>
       </c>
       <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
         <v>0.03</v>
       </c>
-      <c r="V13">
+      <c r="W13">
+        <v>0.01</v>
+      </c>
+      <c r="X13">
         <v>0.12</v>
       </c>
     </row>
@@ -1461,13 +1543,13 @@
         </is>
       </c>
       <c r="G14">
-        <v>0.432</v>
+        <v>0.427</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0.131</v>
+        <v>0.129</v>
       </c>
       <c r="J14">
         <v>0.004</v>
@@ -1479,33 +1561,39 @@
         <v>0.013</v>
       </c>
       <c r="M14">
-        <v>0.42</v>
+        <v>0.415</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
         <v>0.06</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
       <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
         <v>0.05</v>
       </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
       <c r="S14">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T14">
         <v>0.01</v>
       </c>
       <c r="U14">
+        <v>0.01</v>
+      </c>
+      <c r="V14">
         <v>0.18</v>
       </c>
-      <c r="V14">
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
         <v>0.09</v>
       </c>
     </row>
@@ -1541,13 +1629,13 @@
         </is>
       </c>
       <c r="G15">
-        <v>0.482</v>
+        <v>0.48</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0.195</v>
+        <v>0.194</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1559,33 +1647,39 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <v>0.147</v>
+        <v>0.146</v>
       </c>
       <c r="N15">
-        <v>0.177</v>
+        <v>0.004</v>
       </c>
       <c r="O15">
+        <v>0.176</v>
+      </c>
+      <c r="P15">
         <v>0.06</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
       <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <v>0.05</v>
       </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
       <c r="S15">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T15">
         <v>0.01</v>
       </c>
       <c r="U15">
+        <v>0.01</v>
+      </c>
+      <c r="V15">
         <v>0.18</v>
       </c>
-      <c r="V15">
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
         <v>0.09</v>
       </c>
     </row>
@@ -1621,7 +1715,7 @@
         </is>
       </c>
       <c r="G16">
-        <v>0.357</v>
+        <v>0.355</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1639,33 +1733,39 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <v>0.483</v>
+        <v>0.481</v>
       </c>
       <c r="N16">
+        <v>0.005</v>
+      </c>
+      <c r="O16">
+        <v>0.049</v>
+      </c>
+      <c r="P16">
+        <v>0.06</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
         <v>0.05</v>
       </c>
-      <c r="O16">
-        <v>0.06</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0.05</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
       <c r="S16">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T16">
         <v>0.01</v>
       </c>
       <c r="U16">
+        <v>0.01</v>
+      </c>
+      <c r="V16">
         <v>0.18</v>
       </c>
-      <c r="V16">
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
         <v>0.09</v>
       </c>
     </row>
@@ -1725,11 +1825,11 @@
         <v>0</v>
       </c>
       <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>0.09</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
       <c r="Q17">
         <v>0</v>
       </c>
@@ -1743,9 +1843,15 @@
         <v>0</v>
       </c>
       <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>0.1</v>
       </c>
-      <c r="V17">
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
         <v>0</v>
       </c>
     </row>
@@ -1805,11 +1911,11 @@
         <v>0</v>
       </c>
       <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
         <v>0.09</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
       <c r="Q18">
         <v>0</v>
       </c>
@@ -1823,9 +1929,15 @@
         <v>0</v>
       </c>
       <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
         <v>0.1</v>
       </c>
-      <c r="V18">
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
         <v>0</v>
       </c>
     </row>
@@ -1861,7 +1973,7 @@
         </is>
       </c>
       <c r="G19">
-        <v>0.216</v>
+        <v>0.214</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1879,17 +1991,17 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0.775</v>
+        <v>0.769</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <v>0.09</v>
       </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
       <c r="Q19">
         <v>0</v>
       </c>
@@ -1903,9 +2015,15 @@
         <v>0</v>
       </c>
       <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
         <v>0.1</v>
       </c>
-      <c r="V19">
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
         <v>0</v>
       </c>
     </row>
@@ -1941,43 +2059,43 @@
         </is>
       </c>
       <c r="G20">
-        <v>0.386</v>
+        <v>0.368</v>
       </c>
       <c r="H20">
         <v>0.013</v>
       </c>
       <c r="I20">
-        <v>0.541</v>
+        <v>0.517</v>
       </c>
       <c r="J20">
         <v>0.001</v>
       </c>
       <c r="K20">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="L20">
+        <v>0.022</v>
+      </c>
+      <c r="M20">
         <v>0.023</v>
       </c>
-      <c r="M20">
-        <v>0.024</v>
-      </c>
       <c r="N20">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="O20">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
         <v>0.05</v>
       </c>
-      <c r="R20">
-        <v>0</v>
-      </c>
       <c r="S20">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T20">
         <v>0.01</v>
@@ -1986,6 +2104,12 @@
         <v>0.01</v>
       </c>
       <c r="V20">
+        <v>0.01</v>
+      </c>
+      <c r="W20">
+        <v>0.01</v>
+      </c>
+      <c r="X20">
         <v>0</v>
       </c>
     </row>
@@ -2021,13 +2145,13 @@
         </is>
       </c>
       <c r="G21">
-        <v>0.366</v>
+        <v>0.354</v>
       </c>
       <c r="H21">
         <v>0.014</v>
       </c>
       <c r="I21">
-        <v>0.604</v>
+        <v>0.584</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -2039,25 +2163,25 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="N21">
+        <v>0.033</v>
+      </c>
+      <c r="O21">
         <v>0.001</v>
       </c>
-      <c r="O21">
-        <v>0.03</v>
-      </c>
       <c r="P21">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
         <v>0.05</v>
       </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
       <c r="S21">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T21">
         <v>0.01</v>
@@ -2066,6 +2190,12 @@
         <v>0.01</v>
       </c>
       <c r="V21">
+        <v>0.01</v>
+      </c>
+      <c r="W21">
+        <v>0.01</v>
+      </c>
+      <c r="X21">
         <v>0</v>
       </c>
     </row>
@@ -2101,13 +2231,13 @@
         </is>
       </c>
       <c r="G22">
-        <v>0.329</v>
+        <v>0.322</v>
       </c>
       <c r="H22">
         <v>0.008</v>
       </c>
       <c r="I22">
-        <v>0.637</v>
+        <v>0.624</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -2119,25 +2249,25 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="N22">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="O22">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
         <v>0.05</v>
       </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
       <c r="S22">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T22">
         <v>0.01</v>
@@ -2146,6 +2276,12 @@
         <v>0.01</v>
       </c>
       <c r="V22">
+        <v>0.01</v>
+      </c>
+      <c r="W22">
+        <v>0.01</v>
+      </c>
+      <c r="X22">
         <v>0</v>
       </c>
     </row>
@@ -2181,13 +2317,13 @@
         </is>
       </c>
       <c r="G23">
-        <v>0.448</v>
+        <v>0.438</v>
       </c>
       <c r="H23">
         <v>0.016</v>
       </c>
       <c r="I23">
-        <v>0.493</v>
+        <v>0.482</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -2199,23 +2335,23 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>0.042</v>
+        <v>0.041</v>
       </c>
       <c r="N23">
+        <v>0.022</v>
+      </c>
+      <c r="O23">
         <v>0.001</v>
       </c>
-      <c r="O23">
-        <v>0.06</v>
-      </c>
       <c r="P23">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
       <c r="S23">
         <v>0</v>
       </c>
@@ -2223,9 +2359,15 @@
         <v>0</v>
       </c>
       <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>0.02</v>
       </c>
-      <c r="V23">
+      <c r="W23">
+        <v>0.01</v>
+      </c>
+      <c r="X23">
         <v>0</v>
       </c>
     </row>
@@ -2261,13 +2403,13 @@
         </is>
       </c>
       <c r="G24">
-        <v>0.468</v>
+        <v>0.464</v>
       </c>
       <c r="H24">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="I24">
-        <v>0.496</v>
+        <v>0.491</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -2282,20 +2424,20 @@
         <v>0.012</v>
       </c>
       <c r="N24">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="O24">
         <v>0.007</v>
       </c>
-      <c r="O24">
-        <v>0.06</v>
-      </c>
       <c r="P24">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R24">
-        <v>0</v>
-      </c>
       <c r="S24">
         <v>0</v>
       </c>
@@ -2303,9 +2445,15 @@
         <v>0</v>
       </c>
       <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>0.02</v>
       </c>
-      <c r="V24">
+      <c r="W24">
+        <v>0.01</v>
+      </c>
+      <c r="X24">
         <v>0</v>
       </c>
     </row>
@@ -2341,13 +2489,13 @@
         </is>
       </c>
       <c r="G25">
-        <v>0.361</v>
+        <v>0.36</v>
       </c>
       <c r="H25">
         <v>0.016</v>
       </c>
       <c r="I25">
-        <v>0.611</v>
+        <v>0.609</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -2362,20 +2510,20 @@
         <v>0.002</v>
       </c>
       <c r="N25">
+        <v>0.003</v>
+      </c>
+      <c r="O25">
         <v>0.006</v>
       </c>
-      <c r="O25">
-        <v>0.06</v>
-      </c>
       <c r="P25">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
       <c r="S25">
         <v>0</v>
       </c>
@@ -2383,9 +2531,15 @@
         <v>0</v>
       </c>
       <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
         <v>0.02</v>
       </c>
-      <c r="V25">
+      <c r="W25">
+        <v>0.01</v>
+      </c>
+      <c r="X25">
         <v>0</v>
       </c>
     </row>
@@ -2421,13 +2575,13 @@
         </is>
       </c>
       <c r="G26">
-        <v>0.309</v>
+        <v>0.301</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0.092</v>
+        <v>0.09</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -2439,33 +2593,39 @@
         <v>0.015</v>
       </c>
       <c r="M26">
-        <v>0.523</v>
+        <v>0.509</v>
       </c>
       <c r="N26">
-        <v>0.061</v>
+        <v>0.026</v>
       </c>
       <c r="O26">
+        <v>0.06</v>
+      </c>
+      <c r="P26">
         <v>0.03</v>
       </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
       <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
         <v>0.1</v>
       </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
       <c r="S26">
         <v>0</v>
       </c>
       <c r="T26">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U26">
+        <v>0.01</v>
+      </c>
+      <c r="V26">
         <v>0.12</v>
       </c>
-      <c r="V26">
+      <c r="W26">
+        <v>0.01</v>
+      </c>
+      <c r="X26">
         <v>0.02</v>
       </c>
     </row>
@@ -2501,13 +2661,13 @@
         </is>
       </c>
       <c r="G27">
-        <v>0.36</v>
+        <v>0.355</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0.291</v>
+        <v>0.287</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -2519,33 +2679,39 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <v>0.288</v>
+        <v>0.284</v>
       </c>
       <c r="N27">
-        <v>0.061</v>
+        <v>0.013</v>
       </c>
       <c r="O27">
+        <v>0.06</v>
+      </c>
+      <c r="P27">
         <v>0.03</v>
       </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
       <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
         <v>0.1</v>
       </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
       <c r="S27">
         <v>0</v>
       </c>
       <c r="T27">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U27">
+        <v>0.01</v>
+      </c>
+      <c r="V27">
         <v>0.12</v>
       </c>
-      <c r="V27">
+      <c r="W27">
+        <v>0.01</v>
+      </c>
+      <c r="X27">
         <v>0.02</v>
       </c>
     </row>
@@ -2602,30 +2768,36 @@
         <v>0.457</v>
       </c>
       <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
         <v>0.018</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.03</v>
       </c>
-      <c r="P28">
-        <v>0</v>
-      </c>
       <c r="Q28">
+        <v>0</v>
+      </c>
+      <c r="R28">
         <v>0.1</v>
       </c>
-      <c r="R28">
-        <v>0</v>
-      </c>
       <c r="S28">
         <v>0</v>
       </c>
       <c r="T28">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U28">
+        <v>0.01</v>
+      </c>
+      <c r="V28">
         <v>0.12</v>
       </c>
-      <c r="V28">
+      <c r="W28">
+        <v>0.01</v>
+      </c>
+      <c r="X28">
         <v>0.02</v>
       </c>
     </row>
@@ -2661,7 +2833,7 @@
         </is>
       </c>
       <c r="G29">
-        <v>0.762</v>
+        <v>0.757</v>
       </c>
       <c r="H29">
         <v>0.025</v>
@@ -2679,23 +2851,23 @@
         <v>0.003</v>
       </c>
       <c r="M29">
-        <v>0.107</v>
+        <v>0.106</v>
       </c>
       <c r="N29">
+        <v>0.006</v>
+      </c>
+      <c r="O29">
         <v>0.019</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <v>0.05</v>
       </c>
-      <c r="P29">
-        <v>0.01</v>
-      </c>
       <c r="Q29">
+        <v>0.01</v>
+      </c>
+      <c r="R29">
         <v>0.05</v>
       </c>
-      <c r="R29">
-        <v>0</v>
-      </c>
       <c r="S29">
         <v>0</v>
       </c>
@@ -2703,9 +2875,15 @@
         <v>0</v>
       </c>
       <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
         <v>0.03</v>
       </c>
-      <c r="V29">
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
         <v>0.02</v>
       </c>
     </row>
@@ -2741,13 +2919,13 @@
         </is>
       </c>
       <c r="G30">
-        <v>0.697</v>
+        <v>0.693</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30">
-        <v>0.177</v>
+        <v>0.176</v>
       </c>
       <c r="J30">
         <v>0.002</v>
@@ -2759,23 +2937,23 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>0.118</v>
+        <v>0.117</v>
       </c>
       <c r="N30">
         <v>0.006</v>
       </c>
       <c r="O30">
+        <v>0.006</v>
+      </c>
+      <c r="P30">
         <v>0.05</v>
       </c>
-      <c r="P30">
-        <v>0.01</v>
-      </c>
       <c r="Q30">
+        <v>0.01</v>
+      </c>
+      <c r="R30">
         <v>0.05</v>
       </c>
-      <c r="R30">
-        <v>0</v>
-      </c>
       <c r="S30">
         <v>0</v>
       </c>
@@ -2783,9 +2961,15 @@
         <v>0</v>
       </c>
       <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
         <v>0.03</v>
       </c>
-      <c r="V30">
+      <c r="W30">
+        <v>0</v>
+      </c>
+      <c r="X30">
         <v>0.02</v>
       </c>
     </row>
@@ -2821,7 +3005,7 @@
         </is>
       </c>
       <c r="G31">
-        <v>0.672</v>
+        <v>0.669</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2842,20 +3026,20 @@
         <v>0.165</v>
       </c>
       <c r="N31">
-        <v>0.05</v>
+        <v>0.005</v>
       </c>
       <c r="O31">
         <v>0.05</v>
       </c>
       <c r="P31">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="Q31">
+        <v>0.01</v>
+      </c>
+      <c r="R31">
         <v>0.05</v>
       </c>
-      <c r="R31">
-        <v>0</v>
-      </c>
       <c r="S31">
         <v>0</v>
       </c>
@@ -2863,9 +3047,15 @@
         <v>0</v>
       </c>
       <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
         <v>0.03</v>
       </c>
-      <c r="V31">
+      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
         <v>0.02</v>
       </c>
     </row>
@@ -2901,13 +3091,13 @@
         </is>
       </c>
       <c r="G32">
-        <v>0.5580000000000001</v>
+        <v>0.5560000000000001</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32">
-        <v>0.394</v>
+        <v>0.393</v>
       </c>
       <c r="J32">
         <v>0.002</v>
@@ -2922,30 +3112,36 @@
         <v>0</v>
       </c>
       <c r="N32">
+        <v>0.004</v>
+      </c>
+      <c r="O32">
         <v>0.003</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>0.04</v>
       </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
       <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
         <v>0.05</v>
       </c>
-      <c r="R32">
-        <v>0</v>
-      </c>
       <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
         <v>0.03</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <v>0.04</v>
       </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
       <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
         <v>0</v>
       </c>
     </row>
@@ -2981,19 +3177,19 @@
         </is>
       </c>
       <c r="G33">
-        <v>0.614</v>
+        <v>0.613</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33">
-        <v>0.297</v>
+        <v>0.296</v>
       </c>
       <c r="J33">
         <v>0</v>
       </c>
       <c r="K33">
-        <v>0.062</v>
+        <v>0.061</v>
       </c>
       <c r="L33">
         <v>0.028</v>
@@ -3002,30 +3198,36 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
         <v>0.04</v>
       </c>
-      <c r="P33">
-        <v>0</v>
-      </c>
       <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
         <v>0.05</v>
       </c>
-      <c r="R33">
-        <v>0</v>
-      </c>
       <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
         <v>0.03</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <v>0.04</v>
       </c>
-      <c r="U33">
-        <v>0</v>
-      </c>
       <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
         <v>0</v>
       </c>
     </row>
@@ -3061,13 +3263,13 @@
         </is>
       </c>
       <c r="G34">
-        <v>0.531</v>
+        <v>0.528</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34">
-        <v>0.365</v>
+        <v>0.363</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -3082,30 +3284,36 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
         <v>0.04</v>
       </c>
-      <c r="P34">
-        <v>0</v>
-      </c>
       <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
         <v>0.05</v>
       </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
       <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
         <v>0.03</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <v>0.04</v>
       </c>
-      <c r="U34">
-        <v>0</v>
-      </c>
       <c r="V34">
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
         <v>0</v>
       </c>
     </row>
@@ -3141,13 +3349,13 @@
         </is>
       </c>
       <c r="G35">
-        <v>0.645</v>
+        <v>0.637</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35">
-        <v>0.292</v>
+        <v>0.289</v>
       </c>
       <c r="J35">
         <v>0.003</v>
@@ -3162,30 +3370,36 @@
         <v>0.011</v>
       </c>
       <c r="N35">
+        <v>0.013</v>
+      </c>
+      <c r="O35">
         <v>0.014</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>0.02</v>
       </c>
-      <c r="P35">
-        <v>0</v>
-      </c>
       <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
         <v>0.04</v>
       </c>
-      <c r="R35">
-        <v>0</v>
-      </c>
       <c r="S35">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T35">
+        <v>0.01</v>
+      </c>
+      <c r="U35">
         <v>0.03</v>
       </c>
-      <c r="U35">
-        <v>0.01</v>
-      </c>
       <c r="V35">
+        <v>0.01</v>
+      </c>
+      <c r="W35">
+        <v>0.01</v>
+      </c>
+      <c r="X35">
         <v>0.01</v>
       </c>
     </row>
@@ -3221,13 +3435,13 @@
         </is>
       </c>
       <c r="G36">
-        <v>0.619</v>
+        <v>0.61</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36">
-        <v>0.27</v>
+        <v>0.266</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -3236,36 +3450,42 @@
         <v>0.007</v>
       </c>
       <c r="L36">
-        <v>0.096</v>
+        <v>0.094</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
       <c r="N36">
+        <v>0.015</v>
+      </c>
+      <c r="O36">
         <v>0.008</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>0.02</v>
       </c>
-      <c r="P36">
-        <v>0</v>
-      </c>
       <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
         <v>0.04</v>
       </c>
-      <c r="R36">
-        <v>0</v>
-      </c>
       <c r="S36">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T36">
+        <v>0.01</v>
+      </c>
+      <c r="U36">
         <v>0.03</v>
       </c>
-      <c r="U36">
-        <v>0.01</v>
-      </c>
       <c r="V36">
+        <v>0.01</v>
+      </c>
+      <c r="W36">
+        <v>0.01</v>
+      </c>
+      <c r="X36">
         <v>0.01</v>
       </c>
     </row>
@@ -3301,7 +3521,7 @@
         </is>
       </c>
       <c r="G37">
-        <v>0.598</v>
+        <v>0.597</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -3322,30 +3542,36 @@
         <v>0.005</v>
       </c>
       <c r="N37">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
         <v>0.02</v>
       </c>
-      <c r="P37">
-        <v>0</v>
-      </c>
       <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
         <v>0.04</v>
       </c>
-      <c r="R37">
-        <v>0</v>
-      </c>
       <c r="S37">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T37">
+        <v>0.01</v>
+      </c>
+      <c r="U37">
         <v>0.03</v>
       </c>
-      <c r="U37">
-        <v>0.01</v>
-      </c>
       <c r="V37">
+        <v>0.01</v>
+      </c>
+      <c r="W37">
+        <v>0.01</v>
+      </c>
+      <c r="X37">
         <v>0.01</v>
       </c>
     </row>
@@ -3387,7 +3613,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>0.355</v>
+        <v>0.354</v>
       </c>
       <c r="J38">
         <v>0.031</v>
@@ -3402,30 +3628,36 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
       <c r="O38">
+        <v>0.01</v>
+      </c>
+      <c r="P38">
         <v>0.03</v>
       </c>
-      <c r="P38">
-        <v>0</v>
-      </c>
       <c r="Q38">
+        <v>0</v>
+      </c>
+      <c r="R38">
         <v>0.08</v>
       </c>
-      <c r="R38">
-        <v>0.01</v>
-      </c>
       <c r="S38">
+        <v>0.01</v>
+      </c>
+      <c r="T38">
         <v>0.11</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <v>0.04</v>
       </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
       <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
         <v>0.01</v>
       </c>
     </row>
@@ -3485,27 +3717,33 @@
         <v>0</v>
       </c>
       <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
         <v>0.03</v>
       </c>
-      <c r="P39">
-        <v>0</v>
-      </c>
       <c r="Q39">
+        <v>0</v>
+      </c>
+      <c r="R39">
         <v>0.08</v>
       </c>
-      <c r="R39">
-        <v>0.01</v>
-      </c>
       <c r="S39">
+        <v>0.01</v>
+      </c>
+      <c r="T39">
         <v>0.11</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <v>0.04</v>
       </c>
-      <c r="U39">
-        <v>0</v>
-      </c>
       <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
         <v>0.01</v>
       </c>
     </row>
@@ -3541,7 +3779,7 @@
         </is>
       </c>
       <c r="G40">
-        <v>0.415</v>
+        <v>0.414</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3553,7 +3791,7 @@
         <v>0.013</v>
       </c>
       <c r="K40">
-        <v>0.248</v>
+        <v>0.247</v>
       </c>
       <c r="L40">
         <v>0.074</v>
@@ -3562,30 +3800,36 @@
         <v>0</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
         <v>0.03</v>
       </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
       <c r="Q40">
+        <v>0</v>
+      </c>
+      <c r="R40">
         <v>0.08</v>
       </c>
-      <c r="R40">
-        <v>0.01</v>
-      </c>
       <c r="S40">
+        <v>0.01</v>
+      </c>
+      <c r="T40">
         <v>0.11</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <v>0.04</v>
       </c>
-      <c r="U40">
-        <v>0</v>
-      </c>
       <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0</v>
+      </c>
+      <c r="X40">
         <v>0.01</v>
       </c>
     </row>
@@ -3642,30 +3886,36 @@
         <v>0</v>
       </c>
       <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
         <v>0.006</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>0.08</v>
       </c>
-      <c r="P41">
-        <v>0.01</v>
-      </c>
       <c r="Q41">
+        <v>0.01</v>
+      </c>
+      <c r="R41">
         <v>0.08</v>
       </c>
-      <c r="R41">
-        <v>0</v>
-      </c>
       <c r="S41">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T41">
+        <v>0.01</v>
+      </c>
+      <c r="U41">
         <v>0.04</v>
       </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
       <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>0</v>
+      </c>
+      <c r="X41">
         <v>0</v>
       </c>
     </row>
@@ -3722,30 +3972,36 @@
         <v>0</v>
       </c>
       <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
         <v>0.001</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>0.08</v>
       </c>
-      <c r="P42">
-        <v>0.01</v>
-      </c>
       <c r="Q42">
+        <v>0.01</v>
+      </c>
+      <c r="R42">
         <v>0.08</v>
       </c>
-      <c r="R42">
-        <v>0</v>
-      </c>
       <c r="S42">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T42">
+        <v>0.01</v>
+      </c>
+      <c r="U42">
         <v>0.04</v>
       </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
       <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42">
         <v>0</v>
       </c>
     </row>
@@ -3781,13 +4037,13 @@
         </is>
       </c>
       <c r="G43">
-        <v>0.536</v>
+        <v>0.534</v>
       </c>
       <c r="H43">
         <v>0.008</v>
       </c>
       <c r="I43">
-        <v>0.188</v>
+        <v>0.187</v>
       </c>
       <c r="J43">
         <v>0.002</v>
@@ -3802,30 +4058,36 @@
         <v>0.006</v>
       </c>
       <c r="N43">
+        <v>0.004</v>
+      </c>
+      <c r="O43">
         <v>0.011</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>0.08</v>
       </c>
-      <c r="P43">
-        <v>0.01</v>
-      </c>
       <c r="Q43">
+        <v>0.01</v>
+      </c>
+      <c r="R43">
         <v>0.08</v>
       </c>
-      <c r="R43">
-        <v>0</v>
-      </c>
       <c r="S43">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T43">
+        <v>0.01</v>
+      </c>
+      <c r="U43">
         <v>0.04</v>
       </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
       <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>0</v>
+      </c>
+      <c r="X43">
         <v>0</v>
       </c>
     </row>
@@ -3861,13 +4123,13 @@
         </is>
       </c>
       <c r="G44">
-        <v>0.776</v>
+        <v>0.765</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44">
-        <v>0.197</v>
+        <v>0.195</v>
       </c>
       <c r="J44">
         <v>0.001</v>
@@ -3882,30 +4144,36 @@
         <v>0</v>
       </c>
       <c r="N44">
+        <v>0.013</v>
+      </c>
+      <c r="O44">
         <v>0.001</v>
       </c>
-      <c r="O44">
-        <v>0.1</v>
-      </c>
       <c r="P44">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
         <v>0.09</v>
       </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
       <c r="S44">
         <v>0</v>
       </c>
       <c r="T44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U44">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0.02</v>
+      </c>
+      <c r="X44">
         <v>0</v>
       </c>
     </row>
@@ -3941,13 +4209,13 @@
         </is>
       </c>
       <c r="G45">
-        <v>0.923</v>
+        <v>0.882</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45">
-        <v>0.073</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J45">
         <v>0.001</v>
@@ -3962,30 +4230,36 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>0</v>
+        <v>0.045</v>
       </c>
       <c r="O45">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P45">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
         <v>0.09</v>
       </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
       <c r="S45">
         <v>0</v>
       </c>
       <c r="T45">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U45">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0.02</v>
+      </c>
+      <c r="X45">
         <v>0</v>
       </c>
     </row>
@@ -4021,13 +4295,13 @@
         </is>
       </c>
       <c r="G46">
-        <v>0.741</v>
+        <v>0.716</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46">
-        <v>0.254</v>
+        <v>0.245</v>
       </c>
       <c r="J46">
         <v>0.004</v>
@@ -4042,30 +4316,36 @@
         <v>0.002</v>
       </c>
       <c r="N46">
-        <v>0</v>
+        <v>0.033</v>
       </c>
       <c r="O46">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="P46">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
         <v>0.09</v>
       </c>
-      <c r="R46">
-        <v>0</v>
-      </c>
       <c r="S46">
         <v>0</v>
       </c>
       <c r="T46">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U46">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0.02</v>
+      </c>
+      <c r="X46">
         <v>0</v>
       </c>
     </row>
@@ -4101,13 +4381,13 @@
         </is>
       </c>
       <c r="G47">
-        <v>0.493</v>
+        <v>0.482</v>
       </c>
       <c r="H47">
-        <v>0.134</v>
+        <v>0.13</v>
       </c>
       <c r="I47">
-        <v>0.034</v>
+        <v>0.033</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -4116,23 +4396,23 @@
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0.162</v>
+        <v>0.158</v>
       </c>
       <c r="M47">
-        <v>0.177</v>
+        <v>0.172</v>
       </c>
       <c r="N47">
-        <v>0</v>
+        <v>0.024</v>
       </c>
       <c r="O47">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="P47">
+        <v>0.21</v>
+      </c>
+      <c r="Q47">
         <v>0.08</v>
       </c>
-      <c r="Q47">
-        <v>0</v>
-      </c>
       <c r="R47">
         <v>0</v>
       </c>
@@ -4140,12 +4420,18 @@
         <v>0</v>
       </c>
       <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
         <v>0.08</v>
       </c>
-      <c r="U47">
-        <v>0.29</v>
-      </c>
       <c r="V47">
+        <v>0.28</v>
+      </c>
+      <c r="W47">
+        <v>0.01</v>
+      </c>
+      <c r="X47">
         <v>0.01</v>
       </c>
     </row>
@@ -4181,7 +4467,7 @@
         </is>
       </c>
       <c r="G48">
-        <v>0.333</v>
+        <v>0.326</v>
       </c>
       <c r="H48">
         <v>0.005</v>
@@ -4196,23 +4482,23 @@
         <v>0</v>
       </c>
       <c r="L48">
-        <v>0.047</v>
+        <v>0.046</v>
       </c>
       <c r="M48">
-        <v>0.576</v>
+        <v>0.566</v>
       </c>
       <c r="N48">
+        <v>0.019</v>
+      </c>
+      <c r="O48">
         <v>0.008999999999999999</v>
       </c>
-      <c r="O48">
-        <v>0.22</v>
-      </c>
       <c r="P48">
+        <v>0.21</v>
+      </c>
+      <c r="Q48">
         <v>0.08</v>
       </c>
-      <c r="Q48">
-        <v>0</v>
-      </c>
       <c r="R48">
         <v>0</v>
       </c>
@@ -4220,12 +4506,18 @@
         <v>0</v>
       </c>
       <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
         <v>0.08</v>
       </c>
-      <c r="U48">
-        <v>0.29</v>
-      </c>
       <c r="V48">
+        <v>0.28</v>
+      </c>
+      <c r="W48">
+        <v>0.01</v>
+      </c>
+      <c r="X48">
         <v>0.01</v>
       </c>
     </row>
@@ -4261,13 +4553,13 @@
         </is>
       </c>
       <c r="G49">
-        <v>0.765</v>
+        <v>0.733</v>
       </c>
       <c r="H49">
-        <v>0.151</v>
+        <v>0.145</v>
       </c>
       <c r="I49">
-        <v>0.038</v>
+        <v>0.036</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -4279,20 +4571,20 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="N49">
-        <v>0.017</v>
+        <v>0.042</v>
       </c>
       <c r="O49">
-        <v>0.22</v>
+        <v>0.016</v>
       </c>
       <c r="P49">
+        <v>0.21</v>
+      </c>
+      <c r="Q49">
         <v>0.08</v>
       </c>
-      <c r="Q49">
-        <v>0</v>
-      </c>
       <c r="R49">
         <v>0</v>
       </c>
@@ -4300,12 +4592,18 @@
         <v>0</v>
       </c>
       <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
         <v>0.08</v>
       </c>
-      <c r="U49">
-        <v>0.29</v>
-      </c>
       <c r="V49">
+        <v>0.28</v>
+      </c>
+      <c r="W49">
+        <v>0.01</v>
+      </c>
+      <c r="X49">
         <v>0.01</v>
       </c>
     </row>
@@ -4341,13 +4639,13 @@
         </is>
       </c>
       <c r="G50">
-        <v>0.354</v>
+        <v>0.337</v>
       </c>
       <c r="H50">
-        <v>0.114</v>
+        <v>0.108</v>
       </c>
       <c r="I50">
-        <v>0.146</v>
+        <v>0.139</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -4359,34 +4657,40 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>0.35</v>
+        <v>0.332</v>
       </c>
       <c r="N50">
-        <v>0.035</v>
+        <v>0.05</v>
       </c>
       <c r="O50">
+        <v>0.033</v>
+      </c>
+      <c r="P50">
         <v>0.21</v>
       </c>
-      <c r="P50">
+      <c r="Q50">
         <v>0.03</v>
       </c>
-      <c r="Q50">
-        <v>0.05</v>
-      </c>
       <c r="R50">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="S50">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T50">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U50">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="V50">
+        <v>0.15</v>
+      </c>
+      <c r="W50">
         <v>0.02</v>
+      </c>
+      <c r="X50">
+        <v>0.01</v>
       </c>
     </row>
     <row r="51">
@@ -4421,13 +4725,13 @@
         </is>
       </c>
       <c r="G51">
-        <v>0.511</v>
+        <v>0.502</v>
       </c>
       <c r="H51">
-        <v>0.122</v>
+        <v>0.119</v>
       </c>
       <c r="I51">
-        <v>0.057</v>
+        <v>0.056</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -4436,37 +4740,43 @@
         <v>0</v>
       </c>
       <c r="L51">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="M51">
-        <v>0.285</v>
+        <v>0.28</v>
       </c>
       <c r="N51">
         <v>0.019</v>
       </c>
       <c r="O51">
+        <v>0.019</v>
+      </c>
+      <c r="P51">
         <v>0.21</v>
       </c>
-      <c r="P51">
+      <c r="Q51">
         <v>0.03</v>
       </c>
-      <c r="Q51">
-        <v>0.05</v>
-      </c>
       <c r="R51">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="S51">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T51">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U51">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="V51">
+        <v>0.15</v>
+      </c>
+      <c r="W51">
         <v>0.02</v>
+      </c>
+      <c r="X51">
+        <v>0.01</v>
       </c>
     </row>
     <row r="52">
@@ -4501,13 +4811,13 @@
         </is>
       </c>
       <c r="G52">
-        <v>0.777</v>
+        <v>0.76</v>
       </c>
       <c r="H52">
-        <v>0.065</v>
+        <v>0.063</v>
       </c>
       <c r="I52">
-        <v>0.08699999999999999</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -4519,34 +4829,40 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="M52">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="N52">
+        <v>0.021</v>
+      </c>
+      <c r="O52">
         <v>0.004</v>
       </c>
-      <c r="O52">
+      <c r="P52">
         <v>0.21</v>
       </c>
-      <c r="P52">
+      <c r="Q52">
         <v>0.03</v>
       </c>
-      <c r="Q52">
-        <v>0.05</v>
-      </c>
       <c r="R52">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="S52">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="T52">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="U52">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="V52">
+        <v>0.15</v>
+      </c>
+      <c r="W52">
         <v>0.02</v>
+      </c>
+      <c r="X52">
+        <v>0.01</v>
       </c>
     </row>
     <row r="53">
@@ -4581,13 +4897,13 @@
         </is>
       </c>
       <c r="G53">
-        <v>0.517</v>
+        <v>0.509</v>
       </c>
       <c r="H53">
-        <v>0.059</v>
+        <v>0.058</v>
       </c>
       <c r="I53">
-        <v>0.286</v>
+        <v>0.281</v>
       </c>
       <c r="J53">
         <v>0.003</v>
@@ -4599,34 +4915,40 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>0.116</v>
+        <v>0.114</v>
       </c>
       <c r="N53">
+        <v>0.016</v>
+      </c>
+      <c r="O53">
+        <v>0.019</v>
+      </c>
+      <c r="P53">
+        <v>0.19</v>
+      </c>
+      <c r="Q53">
+        <v>0.03</v>
+      </c>
+      <c r="R53">
+        <v>0.16</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="V53">
+        <v>0.06</v>
+      </c>
+      <c r="W53">
         <v>0.02</v>
       </c>
-      <c r="O53">
-        <v>0.19</v>
-      </c>
-      <c r="P53">
+      <c r="X53">
         <v>0.03</v>
-      </c>
-      <c r="Q53">
-        <v>0.17</v>
-      </c>
-      <c r="R53">
-        <v>0</v>
-      </c>
-      <c r="S53">
-        <v>0</v>
-      </c>
-      <c r="T53">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="U53">
-        <v>0.06</v>
-      </c>
-      <c r="V53">
-        <v>0.04</v>
       </c>
     </row>
     <row r="54">
@@ -4661,13 +4983,13 @@
         </is>
       </c>
       <c r="G54">
-        <v>0.434</v>
+        <v>0.412</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>0.411</v>
+        <v>0.39</v>
       </c>
       <c r="J54">
         <v>0.002</v>
@@ -4679,34 +5001,40 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>0.08500000000000001</v>
+        <v>0.08</v>
       </c>
       <c r="N54">
-        <v>0.06900000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="O54">
+        <v>0.065</v>
+      </c>
+      <c r="P54">
         <v>0.19</v>
       </c>
-      <c r="P54">
+      <c r="Q54">
         <v>0.03</v>
       </c>
-      <c r="Q54">
-        <v>0.17</v>
-      </c>
       <c r="R54">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="S54">
         <v>0</v>
       </c>
       <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
         <v>0.07000000000000001</v>
       </c>
-      <c r="U54">
+      <c r="V54">
         <v>0.06</v>
       </c>
-      <c r="V54">
-        <v>0.04</v>
+      <c r="W54">
+        <v>0.02</v>
+      </c>
+      <c r="X54">
+        <v>0.03</v>
       </c>
     </row>
     <row r="55">
@@ -4741,13 +5069,13 @@
         </is>
       </c>
       <c r="G55">
-        <v>0.788</v>
+        <v>0.775</v>
       </c>
       <c r="H55">
         <v>0.013</v>
       </c>
       <c r="I55">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -4756,37 +5084,43 @@
         <v>0.006</v>
       </c>
       <c r="L55">
-        <v>0.115</v>
+        <v>0.113</v>
       </c>
       <c r="M55">
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
         <v>0.19</v>
       </c>
-      <c r="P55">
+      <c r="Q55">
         <v>0.03</v>
       </c>
-      <c r="Q55">
-        <v>0.17</v>
-      </c>
       <c r="R55">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="S55">
         <v>0</v>
       </c>
       <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55">
         <v>0.07000000000000001</v>
       </c>
-      <c r="U55">
+      <c r="V55">
         <v>0.06</v>
       </c>
-      <c r="V55">
-        <v>0.04</v>
+      <c r="W55">
+        <v>0.02</v>
+      </c>
+      <c r="X55">
+        <v>0.03</v>
       </c>
     </row>
     <row r="56">
@@ -4821,13 +5155,13 @@
         </is>
       </c>
       <c r="G56">
-        <v>0.549</v>
+        <v>0.529</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
-        <v>0.429</v>
+        <v>0.413</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -4842,19 +5176,19 @@
         <v>0.002</v>
       </c>
       <c r="N56">
+        <v>0.037</v>
+      </c>
+      <c r="O56">
+        <v>0.019</v>
+      </c>
+      <c r="P56">
         <v>0.02</v>
       </c>
-      <c r="O56">
-        <v>0.03</v>
-      </c>
-      <c r="P56">
-        <v>0</v>
-      </c>
       <c r="Q56">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="R56">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="S56">
         <v>0</v>
@@ -4866,6 +5200,12 @@
         <v>0</v>
       </c>
       <c r="V56">
+        <v>0.01</v>
+      </c>
+      <c r="W56">
+        <v>0.01</v>
+      </c>
+      <c r="X56">
         <v>0.01</v>
       </c>
     </row>
@@ -4901,13 +5241,13 @@
         </is>
       </c>
       <c r="G57">
-        <v>0.5620000000000001</v>
+        <v>0.543</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <v>0.421</v>
+        <v>0.407</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -4919,22 +5259,22 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="N57">
+        <v>0.034</v>
+      </c>
+      <c r="O57">
         <v>0.008999999999999999</v>
       </c>
-      <c r="O57">
-        <v>0.03</v>
-      </c>
       <c r="P57">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Q57">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="R57">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="S57">
         <v>0</v>
@@ -4946,6 +5286,12 @@
         <v>0</v>
       </c>
       <c r="V57">
+        <v>0.01</v>
+      </c>
+      <c r="W57">
+        <v>0.01</v>
+      </c>
+      <c r="X57">
         <v>0.01</v>
       </c>
     </row>
@@ -4981,13 +5327,13 @@
         </is>
       </c>
       <c r="G58">
-        <v>0.504</v>
+        <v>0.499</v>
       </c>
       <c r="H58">
         <v>0</v>
       </c>
       <c r="I58">
-        <v>0.449</v>
+        <v>0.444</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -5002,19 +5348,19 @@
         <v>0.012</v>
       </c>
       <c r="N58">
-        <v>0.036</v>
+        <v>0.01</v>
       </c>
       <c r="O58">
-        <v>0.03</v>
+        <v>0.035</v>
       </c>
       <c r="P58">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="Q58">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="R58">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="S58">
         <v>0</v>
@@ -5026,6 +5372,12 @@
         <v>0</v>
       </c>
       <c r="V58">
+        <v>0.01</v>
+      </c>
+      <c r="W58">
+        <v>0.01</v>
+      </c>
+      <c r="X58">
         <v>0.01</v>
       </c>
     </row>
@@ -5061,13 +5413,13 @@
         </is>
       </c>
       <c r="G59">
-        <v>0.761</v>
+        <v>0.729</v>
       </c>
       <c r="H59">
-        <v>0.097</v>
+        <v>0.093</v>
       </c>
       <c r="I59">
-        <v>0.078</v>
+        <v>0.075</v>
       </c>
       <c r="J59">
         <v>0.004</v>
@@ -5076,36 +5428,42 @@
         <v>0</v>
       </c>
       <c r="L59">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="M59">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="N59">
+        <v>0.042</v>
+      </c>
+      <c r="O59">
         <v>0.004</v>
       </c>
-      <c r="O59">
+      <c r="P59">
+        <v>0.04</v>
+      </c>
+      <c r="Q59">
         <v>0.05</v>
       </c>
-      <c r="P59">
-        <v>0.05</v>
-      </c>
-      <c r="Q59">
+      <c r="R59">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R59">
-        <v>0</v>
-      </c>
       <c r="S59">
         <v>0</v>
       </c>
       <c r="T59">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U59">
         <v>0.01</v>
       </c>
       <c r="V59">
+        <v>0.01</v>
+      </c>
+      <c r="W59">
+        <v>0.02</v>
+      </c>
+      <c r="X59">
         <v>0.01</v>
       </c>
     </row>
@@ -5141,13 +5499,13 @@
         </is>
       </c>
       <c r="G60">
-        <v>0.723</v>
+        <v>0.715</v>
       </c>
       <c r="H60">
-        <v>0.027</v>
+        <v>0.026</v>
       </c>
       <c r="I60">
-        <v>0.209</v>
+        <v>0.206</v>
       </c>
       <c r="J60">
         <v>0.002</v>
@@ -5162,30 +5520,36 @@
         <v>0.022</v>
       </c>
       <c r="N60">
+        <v>0.011</v>
+      </c>
+      <c r="O60">
         <v>0.017</v>
       </c>
-      <c r="O60">
+      <c r="P60">
+        <v>0.04</v>
+      </c>
+      <c r="Q60">
         <v>0.05</v>
       </c>
-      <c r="P60">
-        <v>0.05</v>
-      </c>
-      <c r="Q60">
+      <c r="R60">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R60">
-        <v>0</v>
-      </c>
       <c r="S60">
         <v>0</v>
       </c>
       <c r="T60">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U60">
         <v>0.01</v>
       </c>
       <c r="V60">
+        <v>0.01</v>
+      </c>
+      <c r="W60">
+        <v>0.02</v>
+      </c>
+      <c r="X60">
         <v>0.01</v>
       </c>
     </row>
@@ -5221,13 +5585,13 @@
         </is>
       </c>
       <c r="G61">
-        <v>0.822</v>
+        <v>0.796</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <v>0.137</v>
+        <v>0.132</v>
       </c>
       <c r="J61">
         <v>0</v>
@@ -5236,36 +5600,42 @@
         <v>0</v>
       </c>
       <c r="L61">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="M61">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="N61">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="O61">
+        <v>0.008</v>
+      </c>
+      <c r="P61">
+        <v>0.04</v>
+      </c>
+      <c r="Q61">
         <v>0.05</v>
       </c>
-      <c r="P61">
-        <v>0.05</v>
-      </c>
-      <c r="Q61">
+      <c r="R61">
         <v>0.07000000000000001</v>
       </c>
-      <c r="R61">
-        <v>0</v>
-      </c>
       <c r="S61">
         <v>0</v>
       </c>
       <c r="T61">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="U61">
         <v>0.01</v>
       </c>
       <c r="V61">
+        <v>0.01</v>
+      </c>
+      <c r="W61">
+        <v>0.02</v>
+      </c>
+      <c r="X61">
         <v>0.01</v>
       </c>
     </row>
@@ -5301,13 +5671,13 @@
         </is>
       </c>
       <c r="G62">
-        <v>0.646</v>
+        <v>0.632</v>
       </c>
       <c r="H62">
         <v>0.007</v>
       </c>
       <c r="I62">
-        <v>0.294</v>
+        <v>0.287</v>
       </c>
       <c r="J62">
         <v>0</v>
@@ -5319,33 +5689,39 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="N62">
+        <v>0.021</v>
+      </c>
+      <c r="O62">
         <v>0.005</v>
       </c>
-      <c r="O62">
+      <c r="P62">
         <v>0.04</v>
       </c>
-      <c r="P62">
+      <c r="Q62">
+        <v>0.02</v>
+      </c>
+      <c r="R62">
         <v>0.03</v>
       </c>
-      <c r="Q62">
+      <c r="S62">
+        <v>0</v>
+      </c>
+      <c r="T62">
+        <v>0</v>
+      </c>
+      <c r="U62">
+        <v>0</v>
+      </c>
+      <c r="V62">
         <v>0.03</v>
       </c>
-      <c r="R62">
-        <v>0</v>
-      </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-      <c r="T62">
-        <v>0</v>
-      </c>
-      <c r="U62">
-        <v>0.03</v>
-      </c>
-      <c r="V62">
+      <c r="W62">
+        <v>0</v>
+      </c>
+      <c r="X62">
         <v>0</v>
       </c>
     </row>
@@ -5381,13 +5757,13 @@
         </is>
       </c>
       <c r="G63">
-        <v>0.636</v>
+        <v>0.621</v>
       </c>
       <c r="H63">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="I63">
-        <v>0.286</v>
+        <v>0.279</v>
       </c>
       <c r="J63">
         <v>0.003</v>
@@ -5402,30 +5778,36 @@
         <v>0.005</v>
       </c>
       <c r="N63">
+        <v>0.024</v>
+      </c>
+      <c r="O63">
         <v>0.014</v>
       </c>
-      <c r="O63">
+      <c r="P63">
         <v>0.04</v>
       </c>
-      <c r="P63">
+      <c r="Q63">
+        <v>0.02</v>
+      </c>
+      <c r="R63">
         <v>0.03</v>
       </c>
-      <c r="Q63">
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>0</v>
+      </c>
+      <c r="V63">
         <v>0.03</v>
       </c>
-      <c r="R63">
-        <v>0</v>
-      </c>
-      <c r="S63">
-        <v>0</v>
-      </c>
-      <c r="T63">
-        <v>0</v>
-      </c>
-      <c r="U63">
-        <v>0.03</v>
-      </c>
-      <c r="V63">
+      <c r="W63">
+        <v>0</v>
+      </c>
+      <c r="X63">
         <v>0</v>
       </c>
     </row>
@@ -5461,13 +5843,13 @@
         </is>
       </c>
       <c r="G64">
-        <v>0.715</v>
+        <v>0.702</v>
       </c>
       <c r="H64">
         <v>0.043</v>
       </c>
       <c r="I64">
-        <v>0.236</v>
+        <v>0.231</v>
       </c>
       <c r="J64">
         <v>0</v>
@@ -5482,30 +5864,36 @@
         <v>0</v>
       </c>
       <c r="N64">
+        <v>0.018</v>
+      </c>
+      <c r="O64">
         <v>0.006</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <v>0.04</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
+        <v>0.02</v>
+      </c>
+      <c r="R64">
         <v>0.03</v>
       </c>
-      <c r="Q64">
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>0</v>
+      </c>
+      <c r="U64">
+        <v>0</v>
+      </c>
+      <c r="V64">
         <v>0.03</v>
       </c>
-      <c r="R64">
-        <v>0</v>
-      </c>
-      <c r="S64">
-        <v>0</v>
-      </c>
-      <c r="T64">
-        <v>0</v>
-      </c>
-      <c r="U64">
-        <v>0.03</v>
-      </c>
-      <c r="V64">
+      <c r="W64">
+        <v>0</v>
+      </c>
+      <c r="X64">
         <v>0</v>
       </c>
     </row>
@@ -5541,13 +5929,13 @@
         </is>
       </c>
       <c r="G65">
-        <v>0.8129999999999999</v>
+        <v>0.8030000000000001</v>
       </c>
       <c r="H65">
         <v>0</v>
       </c>
       <c r="I65">
-        <v>0.171</v>
+        <v>0.169</v>
       </c>
       <c r="J65">
         <v>0</v>
@@ -5562,20 +5950,20 @@
         <v>0.013</v>
       </c>
       <c r="N65">
+        <v>0.012</v>
+      </c>
+      <c r="O65">
         <v>0.003</v>
       </c>
-      <c r="O65">
+      <c r="P65">
         <v>0.06</v>
       </c>
-      <c r="P65">
-        <v>0</v>
-      </c>
       <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
         <v>0.06</v>
       </c>
-      <c r="R65">
-        <v>0</v>
-      </c>
       <c r="S65">
         <v>0</v>
       </c>
@@ -5583,9 +5971,15 @@
         <v>0</v>
       </c>
       <c r="U65">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V65">
+        <v>0.01</v>
+      </c>
+      <c r="W65">
+        <v>0.01</v>
+      </c>
+      <c r="X65">
         <v>0</v>
       </c>
     </row>
@@ -5621,13 +6015,13 @@
         </is>
       </c>
       <c r="G66">
-        <v>0.888</v>
+        <v>0.885</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
       <c r="I66">
-        <v>0.102</v>
+        <v>0.101</v>
       </c>
       <c r="J66">
         <v>0</v>
@@ -5642,20 +6036,20 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="N66">
+        <v>0.004</v>
+      </c>
+      <c r="O66">
         <v>0.001</v>
       </c>
-      <c r="O66">
+      <c r="P66">
         <v>0.06</v>
       </c>
-      <c r="P66">
-        <v>0</v>
-      </c>
       <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
         <v>0.06</v>
       </c>
-      <c r="R66">
-        <v>0</v>
-      </c>
       <c r="S66">
         <v>0</v>
       </c>
@@ -5663,9 +6057,15 @@
         <v>0</v>
       </c>
       <c r="U66">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V66">
+        <v>0.01</v>
+      </c>
+      <c r="W66">
+        <v>0.01</v>
+      </c>
+      <c r="X66">
         <v>0</v>
       </c>
     </row>
@@ -5701,7 +6101,7 @@
         </is>
       </c>
       <c r="G67">
-        <v>0.923</v>
+        <v>0.921</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -5722,20 +6122,20 @@
         <v>0.025</v>
       </c>
       <c r="N67">
-        <v>0</v>
+        <v>0.002</v>
       </c>
       <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67">
         <v>0.06</v>
       </c>
-      <c r="P67">
-        <v>0</v>
-      </c>
       <c r="Q67">
+        <v>0</v>
+      </c>
+      <c r="R67">
         <v>0.06</v>
       </c>
-      <c r="R67">
-        <v>0</v>
-      </c>
       <c r="S67">
         <v>0</v>
       </c>
@@ -5743,9 +6143,15 @@
         <v>0</v>
       </c>
       <c r="U67">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V67">
+        <v>0.01</v>
+      </c>
+      <c r="W67">
+        <v>0.01</v>
+      </c>
+      <c r="X67">
         <v>0</v>
       </c>
     </row>
@@ -5787,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <v>0.992</v>
+        <v>0.965</v>
       </c>
       <c r="J68">
         <v>0</v>
@@ -5802,20 +6208,20 @@
         <v>0</v>
       </c>
       <c r="N68">
+        <v>0.027</v>
+      </c>
+      <c r="O68">
         <v>0.008</v>
       </c>
-      <c r="O68">
+      <c r="P68">
+        <v>0.3</v>
+      </c>
+      <c r="Q68">
+        <v>0</v>
+      </c>
+      <c r="R68">
         <v>0.31</v>
       </c>
-      <c r="P68">
-        <v>0</v>
-      </c>
-      <c r="Q68">
-        <v>0.32</v>
-      </c>
-      <c r="R68">
-        <v>0</v>
-      </c>
       <c r="S68">
         <v>0</v>
       </c>
@@ -5823,9 +6229,15 @@
         <v>0</v>
       </c>
       <c r="U68">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V68">
+        <v>0.01</v>
+      </c>
+      <c r="W68">
+        <v>0.02</v>
+      </c>
+      <c r="X68">
         <v>0</v>
       </c>
     </row>
@@ -5861,13 +6273,13 @@
         </is>
       </c>
       <c r="G69">
-        <v>0.524</v>
+        <v>0.5</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
-        <v>0.459</v>
+        <v>0.437</v>
       </c>
       <c r="J69">
         <v>0</v>
@@ -5882,20 +6294,20 @@
         <v>0.014</v>
       </c>
       <c r="N69">
+        <v>0.046</v>
+      </c>
+      <c r="O69">
         <v>0.003</v>
       </c>
-      <c r="O69">
+      <c r="P69">
+        <v>0.3</v>
+      </c>
+      <c r="Q69">
+        <v>0</v>
+      </c>
+      <c r="R69">
         <v>0.31</v>
       </c>
-      <c r="P69">
-        <v>0</v>
-      </c>
-      <c r="Q69">
-        <v>0.32</v>
-      </c>
-      <c r="R69">
-        <v>0</v>
-      </c>
       <c r="S69">
         <v>0</v>
       </c>
@@ -5903,9 +6315,15 @@
         <v>0</v>
       </c>
       <c r="U69">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V69">
+        <v>0.01</v>
+      </c>
+      <c r="W69">
+        <v>0.02</v>
+      </c>
+      <c r="X69">
         <v>0</v>
       </c>
     </row>
@@ -5941,13 +6359,13 @@
         </is>
       </c>
       <c r="G70">
-        <v>0.55</v>
+        <v>0.547</v>
       </c>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="I70">
-        <v>0.424</v>
+        <v>0.422</v>
       </c>
       <c r="J70">
         <v>0.002</v>
@@ -5962,20 +6380,20 @@
         <v>0.021</v>
       </c>
       <c r="N70">
+        <v>0.005</v>
+      </c>
+      <c r="O70">
         <v>0.003</v>
       </c>
-      <c r="O70">
+      <c r="P70">
+        <v>0.3</v>
+      </c>
+      <c r="Q70">
+        <v>0</v>
+      </c>
+      <c r="R70">
         <v>0.31</v>
       </c>
-      <c r="P70">
-        <v>0</v>
-      </c>
-      <c r="Q70">
-        <v>0.32</v>
-      </c>
-      <c r="R70">
-        <v>0</v>
-      </c>
       <c r="S70">
         <v>0</v>
       </c>
@@ -5983,9 +6401,15 @@
         <v>0</v>
       </c>
       <c r="U70">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="V70">
+        <v>0.01</v>
+      </c>
+      <c r="W70">
+        <v>0.02</v>
+      </c>
+      <c r="X70">
         <v>0</v>
       </c>
     </row>

</xml_diff>